<commit_message>
Review EIH, BCH, DCHS, CMH, EHS, CHN, SMH
</commit_message>
<xml_diff>
--- a/New files/Bay Care/10201214 Mease Countryside Hospital.xlsx
+++ b/New files/Bay Care/10201214 Mease Countryside Hospital.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74938A0F-10D5-4EFC-A7A6-1B16A23B21D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{402C565C-EDFA-4D3D-B2A0-1DE9353D9279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{DD4182F4-8DAF-4057-BE93-39BFC9F5A1E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F78A36A2-26B5-4ABD-837C-729F0DF9D883}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_Summary" sheetId="1" r:id="rId1"/>
@@ -956,8 +956,8 @@
       <xdr:rowOff>134620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1676400</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
@@ -966,7 +966,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ADED435-3A3C-2FBB-61DF-45E1E9F0BB37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5B2CB85-8296-54A7-07EF-3597283A9918}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1317,14 +1317,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7593743-C7C8-4B6B-BF19-751BC945B165}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0122E092-7C65-49A9-B3CF-DB2CCACFD9E0}">
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
@@ -1332,6 +1333,7 @@
     <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1810,7 +1812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5357BA53-45C7-4E8A-A937-0EB839A6CAEC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60DD814A-A761-4FEF-9E72-2E866EAAF739}">
   <dimension ref="A1:R121"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1945,9 +1947,7 @@
       <c r="Q2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="12">
-        <v>1002915</v>
-      </c>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="37">
@@ -2001,9 +2001,7 @@
       <c r="Q3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="12">
-        <v>1002915</v>
-      </c>
+      <c r="R3" s="12"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="37">
@@ -2057,9 +2055,7 @@
       <c r="Q4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="12">
-        <v>1002915</v>
-      </c>
+      <c r="R4" s="12"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="37">
@@ -2505,9 +2501,7 @@
       <c r="Q12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R12" s="12">
-        <v>1014478</v>
-      </c>
+      <c r="R12" s="12"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="37">
@@ -2561,9 +2555,7 @@
       <c r="Q13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R13" s="12">
-        <v>1014478</v>
-      </c>
+      <c r="R13" s="12"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="37">
@@ -2617,9 +2609,7 @@
       <c r="Q14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R14" s="12">
-        <v>1014478</v>
-      </c>
+      <c r="R14" s="12"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="37">
@@ -2673,9 +2663,7 @@
       <c r="Q15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R15" s="12">
-        <v>1013695</v>
-      </c>
+      <c r="R15" s="12"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="37">
@@ -2729,9 +2717,7 @@
       <c r="Q16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R16" s="12">
-        <v>1013695</v>
-      </c>
+      <c r="R16" s="12"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="37">
@@ -2785,9 +2771,7 @@
       <c r="Q17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R17" s="12">
-        <v>1013695</v>
-      </c>
+      <c r="R17" s="12"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="37">

</xml_diff>